<commit_message>
New functionality: Toggle walls. Fixed a bug with items near blocks sometimes disappearing. Added big ol' movement buttons (totally touchscreen-ready).
</commit_message>
<xml_diff>
--- a/docs/CC Feature List.xlsx
+++ b/docs/CC Feature List.xlsx
@@ -578,7 +578,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -588,9 +588,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -689,7 +687,7 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D5" t="s">
         <v>28</v>
@@ -831,7 +829,7 @@
         <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -863,7 +861,7 @@
         <v>21</v>
       </c>
       <c r="B20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Alpha 0.3.0 - Teeth, Tanks, and the Red Thief have arrived - all enemies are now in the game!
</commit_message>
<xml_diff>
--- a/docs/CC Feature List.xlsx
+++ b/docs/CC Feature List.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="47">
   <si>
     <t>Tile</t>
   </si>
@@ -123,9 +123,6 @@
     <t>Locks</t>
   </si>
   <si>
-    <t>See Enemies</t>
-  </si>
-  <si>
     <t>Tank</t>
   </si>
   <si>
@@ -144,9 +141,6 @@
     <t>Ball</t>
   </si>
   <si>
-    <t>Random</t>
-  </si>
-  <si>
     <t>Teeth</t>
   </si>
   <si>
@@ -160,6 +154,12 @@
   </si>
   <si>
     <t>Invis. Wall</t>
+  </si>
+  <si>
+    <t>Walker</t>
+  </si>
+  <si>
+    <t>(needs testing w/ enemies)</t>
   </si>
 </sst>
 </file>
@@ -588,7 +588,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -636,10 +638,10 @@
         <v>23</v>
       </c>
       <c r="G2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -656,10 +658,10 @@
         <v>23</v>
       </c>
       <c r="G3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -676,10 +678,10 @@
         <v>23</v>
       </c>
       <c r="G4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -696,10 +698,10 @@
         <v>23</v>
       </c>
       <c r="G5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -716,10 +718,10 @@
         <v>32</v>
       </c>
       <c r="G6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -736,10 +738,10 @@
         <v>32</v>
       </c>
       <c r="G7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -750,24 +752,24 @@
         <v>23</v>
       </c>
       <c r="G8" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="H8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B9" t="s">
         <v>23</v>
       </c>
       <c r="G9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -778,10 +780,10 @@
         <v>24</v>
       </c>
       <c r="G10" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -813,7 +815,7 @@
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -831,32 +833,38 @@
       <c r="B16" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B17" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B18" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="C19" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -864,15 +872,15 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>22</v>
       </c>
       <c r="B21" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>18</v>
       </c>
@@ -880,7 +888,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>20</v>
       </c>
@@ -888,7 +896,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>33</v>
       </c>

</xml_diff>